<commit_message>
fix: ppim03 excel baru, letak enrolmen
</commit_message>
<xml_diff>
--- a/public/exports/KOTAK PPIM 03.xlsx
+++ b/public/exports/KOTAK PPIM 03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vault\Project\giret extreme\baru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA04B1-F27B-49FF-90EA-97F806AC8869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0215BE-2E00-4C10-B102-44C4523090DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BORANG PPIM 03-2023" sheetId="1" r:id="rId1"/>
@@ -27,23 +27,27 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miOAm8caLnRm+/j9E8+MDZL5Cm3kw=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="bQpo60dyrtHn6aud/GnggVNWBnI2JfixL7SsHg7nA6M="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+  <si>
+    <t>Borang PPIM 03-2023 (SR)</t>
+  </si>
   <si>
     <t>KEMENTERIAN KESIHATAN MALAYSIA</t>
   </si>
   <si>
+    <t>REKOD SARINGAN DAN INTERVENSI MEROKOK MELALUI PERKHIDMATAN PERGIGIAN SEKOLAH RENDAH</t>
+  </si>
+  <si>
     <t>BULAN</t>
   </si>
   <si>
@@ -95,21 +99,21 @@
     <t>BUKAN PEROKOK</t>
   </si>
   <si>
+    <t>DALAM INTERVENSI</t>
+  </si>
+  <si>
     <t>BILANGAN</t>
   </si>
   <si>
     <t>LELAKI</t>
   </si>
   <si>
-    <t>PEREMBPUAN</t>
+    <t>PEREMPUAN</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>PEREMPUAN</t>
-  </si>
-  <si>
     <t>ROKOK BIASA (R)</t>
   </si>
   <si>
@@ -143,10 +147,16 @@
     <t xml:space="preserve"> PERALIHAN</t>
   </si>
   <si>
+    <t>KKI (SR)</t>
+  </si>
+  <si>
     <t>JUMLAH</t>
   </si>
   <si>
     <t>PENERANGAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) % Ruangan 7, 24 , 28, 32 dan 36 = Bilangan / Kes Baru X 100                </t>
   </si>
   <si>
     <r>
@@ -218,21 +228,6 @@
     <t>3) KKI = Kanak-Kanak Istimewa</t>
   </si>
   <si>
-    <t>DALAM INTERVENSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) % Ruangan 7, 24 , 28, 32 dan 36 = Bilangan / Kes Baru X 100                </t>
-  </si>
-  <si>
-    <t>REKOD SARINGAN DAN INTERVENSI MEROKOK MELALUI PERKHIDMATAN PERGIGIAN SEKOLAH RENDAH</t>
-  </si>
-  <si>
-    <t>Borang PPIM 03-2023 (SR)</t>
-  </si>
-  <si>
-    <t>KKI (SR)</t>
-  </si>
-  <si>
     <t>4) SR = Sekolah Rendah</t>
   </si>
 </sst>
@@ -240,14 +235,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,12 +269,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -375,7 +362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -676,6 +663,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -706,6 +719,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -751,12 +777,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="95">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -778,238 +803,225 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="5" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1255,8 +1267,8 @@
   </sheetPr>
   <dimension ref="A1:AM1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1267,104 +1279,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" customHeight="1">
-      <c r="AI1" s="88" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ1" s="86"/>
-      <c r="AK1" s="86"/>
-      <c r="AL1" s="86"/>
+      <c r="AI1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
       <c r="AI2" s="1"/>
-      <c r="AJ2" s="89"/>
-      <c r="AK2" s="86"/>
-      <c r="AL2" s="86"/>
+      <c r="AJ2" s="73"/>
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
     </row>
     <row r="3" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A3" s="90" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="86"/>
-      <c r="Z3" s="86"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="86"/>
-      <c r="AC3" s="86"/>
-      <c r="AD3" s="86"/>
-      <c r="AE3" s="86"/>
-      <c r="AF3" s="86"/>
-      <c r="AG3" s="86"/>
-      <c r="AH3" s="86"/>
-      <c r="AI3" s="86"/>
-      <c r="AJ3" s="86"/>
-      <c r="AK3" s="86"/>
-      <c r="AL3" s="86"/>
+      <c r="A3" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71"/>
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="71"/>
+      <c r="AK3" s="71"/>
+      <c r="AL3" s="71"/>
       <c r="AM3" s="2"/>
     </row>
     <row r="4" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A4" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="86"/>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="86"/>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
+      <c r="A4" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="71"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71"/>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="71"/>
+      <c r="AL4" s="71"/>
+      <c r="AM4" s="71"/>
     </row>
     <row r="5" spans="1:39" ht="19.5" customHeight="1">
       <c r="A5" s="4"/>
@@ -1378,18 +1390,18 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="86"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="91" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="86"/>
-      <c r="S5" s="93"/>
-      <c r="T5" s="79"/>
+      <c r="M5" s="75" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="71"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="71"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="77"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
@@ -1453,19 +1465,19 @@
     </row>
     <row r="7" spans="1:39" ht="22.5" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="77"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="9"/>
@@ -1481,25 +1493,25 @@
       <c r="AJ7" s="12"/>
       <c r="AK7" s="12"/>
       <c r="AL7" s="13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AM7" s="14"/>
     </row>
     <row r="8" spans="1:39" ht="22.5" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="79"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="84"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="77"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -1513,25 +1525,25 @@
       <c r="W8" s="8"/>
       <c r="AK8" s="12"/>
       <c r="AL8" s="16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AM8" s="14"/>
     </row>
     <row r="9" spans="1:39" ht="22.5" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="79"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="84"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="77"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -1545,25 +1557,25 @@
       <c r="W9" s="8"/>
       <c r="AK9" s="12"/>
       <c r="AL9" s="16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AM9" s="14"/>
     </row>
     <row r="10" spans="1:39" ht="22.5" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="87"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="79"/>
+        <v>11</v>
+      </c>
+      <c r="B10" s="84"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="77"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -1577,7 +1589,7 @@
       <c r="W10" s="8"/>
       <c r="AK10" s="12"/>
       <c r="AL10" s="17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AM10" s="14"/>
     </row>
@@ -1623,218 +1635,218 @@
       <c r="AM11" s="14"/>
     </row>
     <row r="12" spans="1:39" ht="18" customHeight="1">
-      <c r="A12" s="68" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="74" t="s">
+      <c r="A12" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="74" t="s">
+      <c r="B12" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75"/>
-      <c r="S12" s="75"/>
-      <c r="T12" s="75"/>
-      <c r="U12" s="75"/>
-      <c r="V12" s="76"/>
-      <c r="W12" s="74" t="s">
+      <c r="C12" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="X12" s="75"/>
-      <c r="Y12" s="75"/>
-      <c r="Z12" s="76"/>
-      <c r="AA12" s="74" t="s">
+      <c r="D12" s="80"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="AB12" s="75"/>
-      <c r="AC12" s="75"/>
-      <c r="AD12" s="76"/>
-      <c r="AE12" s="74" t="s">
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="80"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="80"/>
+      <c r="V12" s="81"/>
+      <c r="W12" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="AF12" s="75"/>
-      <c r="AG12" s="75"/>
-      <c r="AH12" s="76"/>
-      <c r="AI12" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ12" s="75"/>
-      <c r="AK12" s="75"/>
-      <c r="AL12" s="76"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="81"/>
+      <c r="AA12" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
+      <c r="AD12" s="81"/>
+      <c r="AE12" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF12" s="80"/>
+      <c r="AG12" s="80"/>
+      <c r="AH12" s="81"/>
+      <c r="AI12" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ12" s="80"/>
+      <c r="AK12" s="80"/>
+      <c r="AL12" s="81"/>
       <c r="AM12" s="19"/>
     </row>
     <row r="13" spans="1:39" ht="18" customHeight="1">
-      <c r="A13" s="69"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="95" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="83" t="s">
+      <c r="A13" s="86"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="80" t="s">
+      <c r="D13" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="83" t="s">
+      <c r="E13" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="S13" s="83" t="s">
+      <c r="F13" s="68" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="T13" s="83" t="s">
+      <c r="H13" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="93"/>
+      <c r="O13" s="93"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="U13" s="83" t="s">
+      <c r="S13" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="95" t="s">
+      <c r="T13" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="W13" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="X13" s="83" t="s">
+      <c r="U13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="V13" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="W13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="Y13" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z13" s="95" t="s">
+      <c r="X13" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y13" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AA13" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB13" s="83" t="s">
+      <c r="Z13" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="AC13" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD13" s="95" t="s">
+      <c r="AB13" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC13" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AE13" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF13" s="83" t="s">
+      <c r="AD13" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="AG13" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH13" s="95" t="s">
+      <c r="AF13" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG13" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AI13" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ13" s="83" t="s">
+      <c r="AH13" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="AK13" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL13" s="95" t="s">
+      <c r="AJ13" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK13" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AM13" s="21"/>
+      <c r="AL13" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM13" s="20"/>
     </row>
     <row r="14" spans="1:39" ht="94.5" customHeight="1">
-      <c r="A14" s="70"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="23" t="s">
+      <c r="A14" s="69"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="I14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="J14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="22" t="s">
-        <v>28</v>
+      <c r="K14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="N14" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="O14" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="P14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" s="23" t="s">
+      <c r="O14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="R14" s="84"/>
-      <c r="S14" s="84"/>
-      <c r="T14" s="84"/>
-      <c r="U14" s="84"/>
-      <c r="V14" s="73"/>
-      <c r="W14" s="70"/>
-      <c r="X14" s="84"/>
-      <c r="Y14" s="84"/>
-      <c r="Z14" s="73"/>
-      <c r="AA14" s="70"/>
-      <c r="AB14" s="84"/>
-      <c r="AC14" s="84"/>
-      <c r="AD14" s="73"/>
-      <c r="AE14" s="70"/>
-      <c r="AF14" s="84"/>
-      <c r="AG14" s="84"/>
-      <c r="AH14" s="73"/>
-      <c r="AI14" s="70"/>
-      <c r="AJ14" s="84"/>
-      <c r="AK14" s="84"/>
-      <c r="AL14" s="73"/>
+      <c r="P14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="65"/>
+      <c r="S14" s="65"/>
+      <c r="T14" s="65"/>
+      <c r="U14" s="65"/>
+      <c r="V14" s="67"/>
+      <c r="W14" s="69"/>
+      <c r="X14" s="65"/>
+      <c r="Y14" s="65"/>
+      <c r="Z14" s="67"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="65"/>
+      <c r="AC14" s="65"/>
+      <c r="AD14" s="67"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="65"/>
+      <c r="AG14" s="65"/>
+      <c r="AH14" s="67"/>
+      <c r="AI14" s="69"/>
+      <c r="AJ14" s="65"/>
+      <c r="AK14" s="65"/>
+      <c r="AL14" s="67"/>
       <c r="AM14" s="25"/>
     </row>
     <row r="15" spans="1:39" ht="15" customHeight="1">
@@ -1958,87 +1970,87 @@
       <c r="A16" s="34">
         <v>1</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="62">
+      <c r="B16" s="35"/>
+      <c r="C16" s="36">
         <f t="shared" ref="C16:C23" si="0">SUM(D16:E16)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="63">
-        <f t="shared" ref="D16:D23" si="1">SUM(H16,Y16,AC16,AK16)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="61">
-        <f t="shared" ref="E16:E23" si="2">SUM(M16,Z16,AD16,AL16)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="62">
-        <f t="shared" ref="F16:F23" si="3">SUM(H16,M16)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="37" t="e">
-        <f t="shared" ref="G16:G24" si="4">F16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="38">
-        <f t="shared" ref="H16:H23" si="5">SUM(I16:L16)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="38">
-        <f t="shared" ref="M16:M23" si="6">SUM(N16:Q16)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
+      <c r="D16" s="37">
+        <f>SUM(H16,Y16,AC16,AG16,AK16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" ref="E16:E23" si="1">SUM(M16,Z16,AD16,AH16,AL16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="36">
+        <f t="shared" ref="F16:F23" si="2">SUM(H16,M16)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="38" t="e">
+        <f t="shared" ref="G16:G24" si="3">F16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="39">
+        <f t="shared" ref="H16:H23" si="4">SUM(I16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="39">
+        <f t="shared" ref="M16:M23" si="5">SUM(N16:Q16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
       <c r="V16" s="35"/>
-      <c r="W16" s="39">
-        <f t="shared" ref="W16:W23" si="7">SUM(Y16:Z16)</f>
-        <v>0</v>
-      </c>
-      <c r="X16" s="40" t="e">
-        <f t="shared" ref="X16:X24" si="8">W16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y16" s="36"/>
+      <c r="W16" s="40">
+        <f t="shared" ref="W16:W23" si="6">SUM(Y16:Z16)</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="41" t="e">
+        <f t="shared" ref="X16:X24" si="7">W16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y16" s="37"/>
       <c r="Z16" s="35"/>
-      <c r="AA16" s="39">
-        <f t="shared" ref="AA16:AA23" si="9">SUM(AC16:AD16)</f>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="40" t="e">
-        <f t="shared" ref="AB16:AB24" si="10">AA16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC16" s="36"/>
+      <c r="AA16" s="40">
+        <f t="shared" ref="AA16:AA23" si="8">SUM(AC16:AD16)</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="41" t="e">
+        <f t="shared" ref="AB16:AB24" si="9">AA16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC16" s="37"/>
       <c r="AD16" s="35"/>
-      <c r="AE16" s="39">
-        <f t="shared" ref="AE16:AE23" si="11">SUM(AG16:AH16)</f>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="40" t="e">
-        <f>AE16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG16" s="36"/>
+      <c r="AE16" s="40">
+        <f t="shared" ref="AE16:AE23" si="10">SUM(AG16:AH16)</f>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="41" t="e">
+        <f t="shared" ref="AF16:AF24" si="11">AE16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG16" s="37"/>
       <c r="AH16" s="35"/>
-      <c r="AI16" s="39">
+      <c r="AI16" s="40">
         <f t="shared" ref="AI16:AI23" si="12">SUM(AK16:AL16)</f>
         <v>0</v>
       </c>
-      <c r="AJ16" s="40" t="e">
+      <c r="AJ16" s="41" t="e">
         <f t="shared" ref="AJ16:AJ24" si="13">AI16/C16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK16" s="36"/>
+      <c r="AK16" s="37"/>
       <c r="AL16" s="35"/>
       <c r="AM16" s="33"/>
     </row>
@@ -2046,87 +2058,87 @@
       <c r="A17" s="34">
         <v>2</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="62">
+      <c r="B17" s="35"/>
+      <c r="C17" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="37">
+        <f t="shared" ref="D16:D23" si="14">SUM(H17,Y17,AC17,AG17,AK17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E17" s="61">
+      <c r="F17" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F17" s="62">
+      <c r="G17" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="38">
+        <v>0</v>
+      </c>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="38">
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="39">
+      <c r="X17" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X17" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="35"/>
+      <c r="AA17" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="35"/>
+      <c r="AE17" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC17" s="36"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF17" s="40" t="e">
-        <f t="shared" ref="AF17:AF23" si="14">AE17/C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG17" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG17" s="37"/>
       <c r="AH17" s="35"/>
-      <c r="AI17" s="39">
+      <c r="AI17" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ17" s="40" t="e">
+      <c r="AJ17" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK17" s="36"/>
+      <c r="AK17" s="37"/>
       <c r="AL17" s="35"/>
       <c r="AM17" s="33"/>
     </row>
@@ -2134,87 +2146,87 @@
       <c r="A18" s="34">
         <v>3</v>
       </c>
-      <c r="B18" s="61"/>
-      <c r="C18" s="62">
+      <c r="B18" s="35"/>
+      <c r="C18" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18" s="61">
+      <c r="F18" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="62">
+      <c r="G18" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="38">
+        <v>0</v>
+      </c>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="38">
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="39">
+      <c r="X18" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X18" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC18" s="37"/>
+      <c r="AD18" s="35"/>
+      <c r="AE18" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC18" s="36"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF18" s="40" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG18" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG18" s="37"/>
       <c r="AH18" s="35"/>
-      <c r="AI18" s="39">
+      <c r="AI18" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ18" s="40" t="e">
+      <c r="AJ18" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK18" s="36"/>
+      <c r="AK18" s="37"/>
       <c r="AL18" s="35"/>
       <c r="AM18" s="33"/>
     </row>
@@ -2222,87 +2234,87 @@
       <c r="A19" s="34">
         <v>4</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="62">
+      <c r="B19" s="35"/>
+      <c r="C19" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E19" s="61">
+      <c r="F19" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" s="62">
+      <c r="G19" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="38">
+        <v>0</v>
+      </c>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="38">
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="39">
+      <c r="X19" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="35"/>
+      <c r="AA19" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="35"/>
-      <c r="AA19" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC19" s="37"/>
+      <c r="AD19" s="35"/>
+      <c r="AE19" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC19" s="36"/>
-      <c r="AD19" s="35"/>
-      <c r="AE19" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF19" s="40" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG19" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG19" s="37"/>
       <c r="AH19" s="35"/>
-      <c r="AI19" s="39">
+      <c r="AI19" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ19" s="40" t="e">
+      <c r="AJ19" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK19" s="36"/>
+      <c r="AK19" s="37"/>
       <c r="AL19" s="35"/>
       <c r="AM19" s="33"/>
     </row>
@@ -2310,87 +2322,87 @@
       <c r="A20" s="34">
         <v>5</v>
       </c>
-      <c r="B20" s="61"/>
-      <c r="C20" s="62">
+      <c r="B20" s="35"/>
+      <c r="C20" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E20" s="61">
+      <c r="F20" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" s="62">
+      <c r="G20" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="38">
+        <v>0</v>
+      </c>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="38">
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="39">
+      <c r="X20" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X20" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y20" s="37"/>
+      <c r="Z20" s="35"/>
+      <c r="AA20" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="35"/>
-      <c r="AA20" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC20" s="37"/>
+      <c r="AD20" s="35"/>
+      <c r="AE20" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC20" s="36"/>
-      <c r="AD20" s="35"/>
-      <c r="AE20" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF20" s="40" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG20" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG20" s="37"/>
       <c r="AH20" s="35"/>
-      <c r="AI20" s="39">
+      <c r="AI20" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ20" s="40" t="e">
+      <c r="AJ20" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK20" s="36"/>
+      <c r="AK20" s="37"/>
       <c r="AL20" s="35"/>
       <c r="AM20" s="33"/>
     </row>
@@ -2398,416 +2410,416 @@
       <c r="A21" s="34">
         <v>6</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62">
+      <c r="B21" s="35"/>
+      <c r="C21" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E21" s="61">
+      <c r="F21" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21" s="62">
+      <c r="G21" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="38">
+        <v>0</v>
+      </c>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="38">
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="39">
+      <c r="X21" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X21" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="35"/>
+      <c r="AA21" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB21" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC21" s="37"/>
+      <c r="AD21" s="35"/>
+      <c r="AE21" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="35"/>
-      <c r="AE21" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF21" s="40" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG21" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG21" s="37"/>
       <c r="AH21" s="35"/>
-      <c r="AI21" s="39">
+      <c r="AI21" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ21" s="40" t="e">
+      <c r="AJ21" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK21" s="36"/>
+      <c r="AK21" s="37"/>
       <c r="AL21" s="35"/>
       <c r="AM21" s="33"/>
     </row>
     <row r="22" spans="1:39" ht="34.5" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="62">
+        <v>35</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E22" s="61">
+      <c r="F22" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22" s="62">
+      <c r="G22" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="38">
+        <v>0</v>
+      </c>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="38">
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="39">
+      <c r="X22" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="35"/>
-      <c r="AA22" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC22" s="37"/>
+      <c r="AD22" s="35"/>
+      <c r="AE22" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC22" s="36"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF22" s="40" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG22" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG22" s="37"/>
       <c r="AH22" s="35"/>
-      <c r="AI22" s="39">
+      <c r="AI22" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ22" s="40" t="e">
+      <c r="AJ22" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK22" s="36"/>
+      <c r="AK22" s="37"/>
       <c r="AL22" s="35"/>
       <c r="AM22" s="33"/>
     </row>
     <row r="23" spans="1:39" ht="34.5" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62">
+        <v>36</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D23" s="63">
+      <c r="D23" s="37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E23" s="61">
+      <c r="F23" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="62">
+      <c r="G23" s="38" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="37" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="39">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H23" s="38">
+        <v>0</v>
+      </c>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="38">
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="39">
+      <c r="X23" s="41" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y23" s="37"/>
+      <c r="Z23" s="35"/>
+      <c r="AA23" s="40">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="35"/>
-      <c r="AA23" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="41" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="40" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC23" s="37"/>
+      <c r="AD23" s="35"/>
+      <c r="AE23" s="40">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC23" s="36"/>
-      <c r="AD23" s="35"/>
-      <c r="AE23" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="41" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF23" s="40" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG23" s="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG23" s="37"/>
       <c r="AH23" s="35"/>
-      <c r="AI23" s="39">
+      <c r="AI23" s="40">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ23" s="40" t="e">
+      <c r="AJ23" s="41" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK23" s="36"/>
+      <c r="AK23" s="37"/>
       <c r="AL23" s="35"/>
       <c r="AM23" s="33"/>
     </row>
     <row r="24" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A24" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="42">
+      <c r="A24" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="43">
         <f t="shared" ref="B24:F24" si="15">SUM(B16:B23)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="D24" s="65">
+      <c r="D24" s="45">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="E24" s="66">
+      <c r="E24" s="46">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="F24" s="67">
+      <c r="F24" s="47">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G24" s="45" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="46">
+      <c r="G24" s="48" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="49">
         <f t="shared" ref="H24:W24" si="16">SUM(H16:H23)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="46">
+      <c r="I24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J24" s="46">
+      <c r="J24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="K24" s="46">
+      <c r="K24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="L24" s="46">
+      <c r="L24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N24" s="46">
+      <c r="N24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="O24" s="46">
+      <c r="O24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="P24" s="46">
+      <c r="P24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="46">
+      <c r="Q24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="R24" s="46">
+      <c r="R24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="S24" s="46">
+      <c r="S24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="T24" s="46">
+      <c r="T24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="U24" s="46">
+      <c r="U24" s="49">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="V24" s="43">
+      <c r="V24" s="46">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="W24" s="44">
+      <c r="W24" s="47">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="X24" s="45" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y24" s="46">
+      <c r="X24" s="48" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y24" s="49">
         <f t="shared" ref="Y24:AA24" si="17">SUM(Y16:Y23)</f>
         <v>0</v>
       </c>
-      <c r="Z24" s="43">
+      <c r="Z24" s="46">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AA24" s="44">
+      <c r="AA24" s="47">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB24" s="45" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC24" s="46">
-        <f t="shared" ref="AC24:AI24" si="18">SUM(AC16:AC23)</f>
-        <v>0</v>
-      </c>
-      <c r="AD24" s="43">
+      <c r="AB24" s="48" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC24" s="49">
+        <f t="shared" ref="AC24:AE24" si="18">SUM(AC16:AC23)</f>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="46">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AE24" s="44">
-        <f t="shared" ref="AE24" si="19">SUM(AE16:AE23)</f>
-        <v>0</v>
-      </c>
-      <c r="AF24" s="45" t="e">
-        <f>AE24/C24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG24" s="46">
-        <f t="shared" ref="AG24:AH24" si="20">SUM(AG16:AG23)</f>
-        <v>0</v>
-      </c>
-      <c r="AH24" s="43">
+      <c r="AE24" s="47">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="48" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG24" s="49">
+        <f t="shared" ref="AG24:AI24" si="19">SUM(AG16:AG23)</f>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="46">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="47">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="48" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK24" s="49">
+        <f t="shared" ref="AK24:AL24" si="20">SUM(AK16:AK23)</f>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="46">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AI24" s="44">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="45" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK24" s="46">
-        <f t="shared" ref="AK24:AL24" si="21">SUM(AK16:AK23)</f>
-        <v>0</v>
-      </c>
-      <c r="AL24" s="43">
-        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AM24" s="33" t="e">
@@ -2816,63 +2828,63 @@
       </c>
     </row>
     <row r="25" spans="1:39" ht="15" customHeight="1">
-      <c r="A25" s="47"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="48"/>
-      <c r="R25" s="48"/>
-      <c r="S25" s="48"/>
-      <c r="T25" s="48"/>
-      <c r="U25" s="48"/>
-      <c r="V25" s="48"/>
-      <c r="W25" s="48"/>
-      <c r="X25" s="49"/>
-      <c r="Y25" s="48"/>
-      <c r="Z25" s="48"/>
-      <c r="AA25" s="48"/>
-      <c r="AB25" s="49"/>
-      <c r="AC25" s="48"/>
-      <c r="AD25" s="48"/>
-      <c r="AE25" s="48"/>
-      <c r="AF25" s="48"/>
-      <c r="AG25" s="48"/>
-      <c r="AH25" s="48"/>
-      <c r="AI25" s="48"/>
-      <c r="AJ25" s="49"/>
-      <c r="AK25" s="48"/>
-      <c r="AL25" s="48"/>
-      <c r="AM25" s="50"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="51"/>
+      <c r="W25" s="51"/>
+      <c r="X25" s="52"/>
+      <c r="Y25" s="51"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="51"/>
+      <c r="AB25" s="52"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+      <c r="AE25" s="51"/>
+      <c r="AF25" s="51"/>
+      <c r="AG25" s="51"/>
+      <c r="AH25" s="51"/>
+      <c r="AI25" s="51"/>
+      <c r="AJ25" s="52"/>
+      <c r="AK25" s="51"/>
+      <c r="AL25" s="51"/>
+      <c r="AM25" s="53"/>
     </row>
     <row r="26" spans="1:39">
-      <c r="A26" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
+      <c r="A26" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -2900,22 +2912,22 @@
       <c r="AM26" s="11"/>
     </row>
     <row r="27" spans="1:39">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="53"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -2943,188 +2955,188 @@
       <c r="AM27" s="11"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
+      <c r="A28" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
     </row>
     <row r="29" spans="1:39">
-      <c r="A29" s="54" t="s">
-        <v>37</v>
+      <c r="A29" s="57" t="s">
+        <v>41</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="1:39">
-      <c r="A30" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
+      <c r="A30" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="57"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="54"/>
-      <c r="U30" s="54"/>
-      <c r="V30" s="54"/>
-      <c r="W30" s="54"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="54"/>
-      <c r="Z30" s="54"/>
-      <c r="AA30" s="54"/>
-      <c r="AB30" s="54"/>
-      <c r="AC30" s="54"/>
-      <c r="AD30" s="54"/>
-      <c r="AE30" s="54"/>
-      <c r="AF30" s="54"/>
-      <c r="AG30" s="54"/>
-      <c r="AH30" s="54"/>
-      <c r="AI30" s="58"/>
-      <c r="AJ30" s="58"/>
-      <c r="AK30" s="58"/>
-      <c r="AL30" s="58"/>
-      <c r="AM30" s="58"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="57"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="57"/>
+      <c r="Z30" s="57"/>
+      <c r="AA30" s="57"/>
+      <c r="AB30" s="57"/>
+      <c r="AC30" s="57"/>
+      <c r="AD30" s="57"/>
+      <c r="AE30" s="57"/>
+      <c r="AF30" s="57"/>
+      <c r="AG30" s="57"/>
+      <c r="AH30" s="57"/>
+      <c r="AI30" s="61"/>
+      <c r="AJ30" s="61"/>
+      <c r="AK30" s="61"/>
+      <c r="AL30" s="61"/>
+      <c r="AM30" s="61"/>
     </row>
     <row r="31" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A31" s="54"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-      <c r="P31" s="54"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="54"/>
-      <c r="S31" s="54"/>
-      <c r="T31" s="54"/>
-      <c r="U31" s="54"/>
-      <c r="V31" s="54"/>
-      <c r="W31" s="54"/>
-      <c r="X31" s="54"/>
-      <c r="Y31" s="54"/>
-      <c r="Z31" s="54"/>
-      <c r="AA31" s="54"/>
-      <c r="AB31" s="54"/>
-      <c r="AC31" s="54"/>
-      <c r="AD31" s="54"/>
-      <c r="AE31" s="54"/>
-      <c r="AF31" s="54"/>
-      <c r="AG31" s="54"/>
-      <c r="AH31" s="54"/>
-      <c r="AI31" s="58"/>
-      <c r="AJ31" s="58"/>
-      <c r="AK31" s="58"/>
-      <c r="AL31" s="58"/>
-      <c r="AM31" s="58"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="57"/>
+      <c r="AA31" s="57"/>
+      <c r="AB31" s="57"/>
+      <c r="AC31" s="57"/>
+      <c r="AD31" s="57"/>
+      <c r="AE31" s="57"/>
+      <c r="AF31" s="57"/>
+      <c r="AG31" s="57"/>
+      <c r="AH31" s="57"/>
+      <c r="AI31" s="61"/>
+      <c r="AJ31" s="61"/>
+      <c r="AK31" s="61"/>
+      <c r="AL31" s="61"/>
+      <c r="AM31" s="61"/>
     </row>
     <row r="32" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A32" s="54"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
-      <c r="T32" s="58"/>
-      <c r="U32" s="58"/>
-      <c r="V32" s="58"/>
-      <c r="W32" s="58"/>
-      <c r="X32" s="58"/>
-      <c r="Y32" s="58"/>
-      <c r="Z32" s="58"/>
-      <c r="AA32" s="58"/>
-      <c r="AB32" s="58"/>
-      <c r="AC32" s="58"/>
-      <c r="AD32" s="58"/>
-      <c r="AE32" s="58"/>
-      <c r="AF32" s="58"/>
-      <c r="AG32" s="58"/>
-      <c r="AH32" s="58"/>
-      <c r="AI32" s="58"/>
-      <c r="AJ32" s="58"/>
-      <c r="AK32" s="58"/>
-      <c r="AL32" s="58"/>
-      <c r="AM32" s="58"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="61"/>
+      <c r="S32" s="61"/>
+      <c r="T32" s="61"/>
+      <c r="U32" s="61"/>
+      <c r="V32" s="61"/>
+      <c r="W32" s="61"/>
+      <c r="X32" s="61"/>
+      <c r="Y32" s="61"/>
+      <c r="Z32" s="61"/>
+      <c r="AA32" s="61"/>
+      <c r="AB32" s="61"/>
+      <c r="AC32" s="61"/>
+      <c r="AD32" s="61"/>
+      <c r="AE32" s="61"/>
+      <c r="AF32" s="61"/>
+      <c r="AG32" s="61"/>
+      <c r="AH32" s="61"/>
+      <c r="AI32" s="61"/>
+      <c r="AJ32" s="61"/>
+      <c r="AK32" s="61"/>
+      <c r="AL32" s="61"/>
+      <c r="AM32" s="61"/>
     </row>
     <row r="33" spans="2:29" ht="15" customHeight="1">
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="60"/>
-      <c r="U33" s="60"/>
-      <c r="V33" s="60"/>
-      <c r="W33" s="60"/>
-      <c r="X33" s="60"/>
-      <c r="Y33" s="60"/>
-      <c r="Z33" s="60"/>
-      <c r="AA33" s="60"/>
-      <c r="AB33" s="60"/>
-      <c r="AC33" s="60"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="63"/>
+      <c r="V33" s="63"/>
+      <c r="W33" s="63"/>
+      <c r="X33" s="63"/>
+      <c r="Y33" s="63"/>
+      <c r="Z33" s="63"/>
+      <c r="AA33" s="63"/>
+      <c r="AB33" s="63"/>
+      <c r="AC33" s="63"/>
     </row>
     <row r="34" spans="2:29" ht="15.75" customHeight="1"/>
     <row r="35" spans="2:29" ht="15.75" customHeight="1"/>
@@ -4095,58 +4107,58 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="AE12:AH12"/>
-    <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AG13:AG14"/>
-    <mergeCell ref="AH13:AH14"/>
-    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AB13:AB14"/>
     <mergeCell ref="AL13:AL14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
     <mergeCell ref="W13:W14"/>
     <mergeCell ref="X13:X14"/>
     <mergeCell ref="Y13:Y14"/>
     <mergeCell ref="Z13:Z14"/>
     <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AI13:AI14"/>
-    <mergeCell ref="AJ13:AJ14"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="B9:L9"/>
     <mergeCell ref="B10:L10"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="A3:AL3"/>
     <mergeCell ref="A4:AM4"/>
     <mergeCell ref="O5:P5"/>
-    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="S5:T5"/>
-    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:V12"/>
     <mergeCell ref="W12:Z12"/>
     <mergeCell ref="AA12:AD12"/>
+    <mergeCell ref="AE12:AH12"/>
     <mergeCell ref="AI12:AL12"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:V12"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="M13:Q13"/>
-    <mergeCell ref="R13:R14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="AJ13:AJ14"/>
+    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AG13:AG14"/>
+    <mergeCell ref="AH13:AH14"/>
+    <mergeCell ref="AI13:AI14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.74803149606299213" header="0" footer="0"/>
-  <pageSetup paperSize="8" scale="47" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: buang formula lama dalam excel
</commit_message>
<xml_diff>
--- a/public/exports/KOTAK PPIM 03.xlsx
+++ b/public/exports/KOTAK PPIM 03.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0215BE-2E00-4C10-B102-44C4523090DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B78BE066-C31B-4E52-9F4F-FCD13107B37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BORANG PPIM 03-2023" sheetId="1" r:id="rId1"/>
+    <sheet name="BORANG PPIM 03-2023 (SR)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -240,7 +237,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,11 +289,6 @@
     <font>
       <b/>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -780,14 +772,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -819,27 +808,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -852,31 +832,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,13 +904,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -947,7 +922,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -956,7 +931,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1035,33 +1010,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="SEREMBAN"/>
-      <sheetName val="PD"/>
-      <sheetName val="JEMPOL"/>
-      <sheetName val="TAMPIN"/>
-      <sheetName val="JELEBU"/>
-      <sheetName val="K.PILAH"/>
-      <sheetName val="REMBAU"/>
-      <sheetName val="COMBINED"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1267,1876 +1215,1844 @@
   </sheetPr>
   <dimension ref="A1:AM1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO23" sqref="AO23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="38" width="11.28515625" customWidth="1"/>
-    <col min="39" max="39" width="0.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1">
-      <c r="AI1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ1" s="71"/>
-      <c r="AK1" s="71"/>
-      <c r="AL1" s="71"/>
+    <row r="1" spans="1:38" ht="15" customHeight="1">
+      <c r="AI1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ1" s="64"/>
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="64"/>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1">
+    <row r="2" spans="1:38" ht="15" customHeight="1">
       <c r="AI2" s="1"/>
-      <c r="AJ2" s="73"/>
-      <c r="AK2" s="71"/>
-      <c r="AL2" s="71"/>
+      <c r="AJ2" s="66"/>
+      <c r="AK2" s="64"/>
+      <c r="AL2" s="64"/>
     </row>
-    <row r="3" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A3" s="74" t="s">
+    <row r="3" spans="1:38" ht="19.5" customHeight="1">
+      <c r="A3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="71"/>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="71"/>
-      <c r="Z3" s="71"/>
-      <c r="AA3" s="71"/>
-      <c r="AB3" s="71"/>
-      <c r="AC3" s="71"/>
-      <c r="AD3" s="71"/>
-      <c r="AE3" s="71"/>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="71"/>
-      <c r="AH3" s="71"/>
-      <c r="AI3" s="71"/>
-      <c r="AJ3" s="71"/>
-      <c r="AK3" s="71"/>
-      <c r="AL3" s="71"/>
-      <c r="AM3" s="2"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="64"/>
     </row>
-    <row r="4" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A4" s="75" t="s">
+    <row r="4" spans="1:38" ht="19.5" customHeight="1">
+      <c r="A4" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="71"/>
-      <c r="V4" s="71"/>
-      <c r="W4" s="71"/>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="71"/>
-      <c r="AA4" s="71"/>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="71"/>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="71"/>
-      <c r="AK4" s="71"/>
-      <c r="AL4" s="71"/>
-      <c r="AM4" s="71"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="64"/>
+      <c r="AJ4" s="64"/>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
     </row>
-    <row r="5" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="75" t="s">
+    <row r="5" spans="1:38" ht="19.5" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="71"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="75" t="s">
+      <c r="N5" s="64"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="71"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
-      <c r="AG6" s="6"/>
-      <c r="AH6" s="6"/>
-      <c r="AI6" s="6"/>
-      <c r="AJ6" s="6"/>
-      <c r="AK6" s="6"/>
-      <c r="AL6" s="6"/>
-      <c r="AM6" s="6"/>
+    <row r="6" spans="1:38" ht="15" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
     </row>
-    <row r="7" spans="1:39" ht="22.5" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:38" ht="22.5" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="11"/>
-      <c r="AI7" s="12"/>
-      <c r="AJ7" s="12"/>
-      <c r="AK7" s="12"/>
-      <c r="AL7" s="13" t="s">
+      <c r="B7" s="75"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="10"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AM7" s="14"/>
     </row>
-    <row r="8" spans="1:39" ht="22.5" customHeight="1">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:38" ht="22.5" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="16" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AM8" s="14"/>
     </row>
-    <row r="9" spans="1:39" ht="22.5" customHeight="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:38" ht="22.5" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="AK9" s="12"/>
-      <c r="AL9" s="16" t="s">
+      <c r="B9" s="77"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="AM9" s="14"/>
     </row>
-    <row r="10" spans="1:39" ht="22.5" customHeight="1">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:38" ht="22.5" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="AK10" s="12"/>
-      <c r="AL10" s="17" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AM10" s="14"/>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
-      <c r="AH11" s="18"/>
-      <c r="AI11" s="18"/>
-      <c r="AJ11" s="18"/>
-      <c r="AK11" s="18"/>
-      <c r="AL11" s="18"/>
-      <c r="AM11" s="14"/>
+    <row r="11" spans="1:38" ht="15" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="16"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="16"/>
+      <c r="AH11" s="16"/>
+      <c r="AI11" s="16"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="16"/>
     </row>
-    <row r="12" spans="1:39" ht="18" customHeight="1">
-      <c r="A12" s="85" t="s">
+    <row r="12" spans="1:38" ht="18" customHeight="1">
+      <c r="A12" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="80"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="79" t="s">
+      <c r="D12" s="73"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="80"/>
-      <c r="Q12" s="80"/>
-      <c r="R12" s="80"/>
-      <c r="S12" s="80"/>
-      <c r="T12" s="80"/>
-      <c r="U12" s="80"/>
-      <c r="V12" s="81"/>
-      <c r="W12" s="79" t="s">
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="73"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="X12" s="80"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="81"/>
-      <c r="AA12" s="79" t="s">
+      <c r="X12" s="73"/>
+      <c r="Y12" s="73"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="AB12" s="80"/>
-      <c r="AC12" s="80"/>
-      <c r="AD12" s="81"/>
-      <c r="AE12" s="79" t="s">
+      <c r="AB12" s="73"/>
+      <c r="AC12" s="73"/>
+      <c r="AD12" s="74"/>
+      <c r="AE12" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="AF12" s="80"/>
-      <c r="AG12" s="80"/>
-      <c r="AH12" s="81"/>
-      <c r="AI12" s="79" t="s">
+      <c r="AF12" s="73"/>
+      <c r="AG12" s="73"/>
+      <c r="AH12" s="74"/>
+      <c r="AI12" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="AJ12" s="80"/>
-      <c r="AK12" s="80"/>
-      <c r="AL12" s="81"/>
-      <c r="AM12" s="19"/>
+      <c r="AJ12" s="73"/>
+      <c r="AK12" s="73"/>
+      <c r="AL12" s="74"/>
     </row>
-    <row r="13" spans="1:39" ht="18" customHeight="1">
-      <c r="A13" s="86"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="68" t="s">
+    <row r="13" spans="1:38" ht="18" customHeight="1">
+      <c r="A13" s="79"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="89" t="s">
+      <c r="H13" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="91"/>
-      <c r="M13" s="92" t="s">
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="N13" s="93"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="93"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="64" t="s">
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="S13" s="64" t="s">
+      <c r="S13" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="64" t="s">
+      <c r="T13" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="U13" s="64" t="s">
+      <c r="U13" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="V13" s="66" t="s">
+      <c r="V13" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="W13" s="68" t="s">
+      <c r="W13" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="64" t="s">
+      <c r="X13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="Y13" s="64" t="s">
+      <c r="Y13" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="Z13" s="66" t="s">
+      <c r="Z13" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AA13" s="68" t="s">
+      <c r="AA13" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="AB13" s="64" t="s">
+      <c r="AB13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="AC13" s="64" t="s">
+      <c r="AC13" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="AD13" s="66" t="s">
+      <c r="AD13" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AE13" s="68" t="s">
+      <c r="AE13" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="AF13" s="64" t="s">
+      <c r="AF13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="AG13" s="64" t="s">
+      <c r="AG13" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="AH13" s="66" t="s">
+      <c r="AH13" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AI13" s="68" t="s">
+      <c r="AI13" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="AJ13" s="64" t="s">
+      <c r="AJ13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="AK13" s="64" t="s">
+      <c r="AK13" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="AL13" s="66" t="s">
+      <c r="AL13" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AM13" s="20"/>
     </row>
-    <row r="14" spans="1:39" ht="94.5" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="21" t="s">
+    <row r="14" spans="1:38" ht="94.5" customHeight="1">
+      <c r="A14" s="62"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="M14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N14" s="24" t="s">
+      <c r="N14" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O14" s="22" t="s">
+      <c r="O14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="P14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" s="22" t="s">
+      <c r="Q14" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="R14" s="65"/>
-      <c r="S14" s="65"/>
-      <c r="T14" s="65"/>
-      <c r="U14" s="65"/>
-      <c r="V14" s="67"/>
-      <c r="W14" s="69"/>
-      <c r="X14" s="65"/>
-      <c r="Y14" s="65"/>
-      <c r="Z14" s="67"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="65"/>
-      <c r="AC14" s="65"/>
-      <c r="AD14" s="67"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="65"/>
-      <c r="AG14" s="65"/>
-      <c r="AH14" s="67"/>
-      <c r="AI14" s="69"/>
-      <c r="AJ14" s="65"/>
-      <c r="AK14" s="65"/>
-      <c r="AL14" s="67"/>
-      <c r="AM14" s="25"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="60"/>
+      <c r="AE14" s="62"/>
+      <c r="AF14" s="58"/>
+      <c r="AG14" s="58"/>
+      <c r="AH14" s="60"/>
+      <c r="AI14" s="62"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="58"/>
+      <c r="AL14" s="60"/>
     </row>
-    <row r="15" spans="1:39" ht="15" customHeight="1">
-      <c r="A15" s="26">
+    <row r="15" spans="1:38" ht="15" customHeight="1">
+      <c r="A15" s="21">
         <v>1</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="22">
         <v>2</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="23">
         <v>3</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="24">
         <v>4</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="22">
         <v>5</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="25">
         <v>6</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="26">
         <v>7</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="26">
         <v>8</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="24">
         <v>9</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="24">
         <v>10</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="24">
         <v>11</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="24">
         <v>12</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="27">
         <v>13</v>
       </c>
-      <c r="N15" s="29">
+      <c r="N15" s="24">
         <v>14</v>
       </c>
-      <c r="O15" s="29">
+      <c r="O15" s="24">
         <v>15</v>
       </c>
-      <c r="P15" s="29">
+      <c r="P15" s="24">
         <v>16</v>
       </c>
-      <c r="Q15" s="29">
+      <c r="Q15" s="24">
         <v>17</v>
       </c>
-      <c r="R15" s="29">
+      <c r="R15" s="24">
         <v>18</v>
       </c>
-      <c r="S15" s="29">
+      <c r="S15" s="24">
         <v>19</v>
       </c>
-      <c r="T15" s="29">
+      <c r="T15" s="24">
         <v>20</v>
       </c>
-      <c r="U15" s="29">
+      <c r="U15" s="24">
         <v>21</v>
       </c>
-      <c r="V15" s="27">
+      <c r="V15" s="22">
         <v>22</v>
       </c>
-      <c r="W15" s="28">
+      <c r="W15" s="23">
         <v>23</v>
       </c>
-      <c r="X15" s="29">
+      <c r="X15" s="24">
         <v>24</v>
       </c>
-      <c r="Y15" s="29">
+      <c r="Y15" s="24">
         <v>25</v>
       </c>
-      <c r="Z15" s="27">
+      <c r="Z15" s="22">
         <v>26</v>
       </c>
-      <c r="AA15" s="28">
+      <c r="AA15" s="23">
         <v>27</v>
       </c>
-      <c r="AB15" s="29">
+      <c r="AB15" s="24">
         <v>28</v>
       </c>
-      <c r="AC15" s="29">
+      <c r="AC15" s="24">
         <v>29</v>
       </c>
-      <c r="AD15" s="27">
+      <c r="AD15" s="22">
         <v>30</v>
       </c>
-      <c r="AE15" s="28">
+      <c r="AE15" s="23">
         <v>31</v>
       </c>
-      <c r="AF15" s="29">
+      <c r="AF15" s="24">
         <v>32</v>
       </c>
-      <c r="AG15" s="29">
+      <c r="AG15" s="24">
         <v>33</v>
       </c>
-      <c r="AH15" s="27">
+      <c r="AH15" s="22">
         <v>34</v>
       </c>
-      <c r="AI15" s="28">
+      <c r="AI15" s="23">
         <v>35</v>
       </c>
-      <c r="AJ15" s="29">
+      <c r="AJ15" s="24">
         <v>36</v>
       </c>
-      <c r="AK15" s="29">
+      <c r="AK15" s="24">
         <v>37</v>
       </c>
-      <c r="AL15" s="27">
+      <c r="AL15" s="22">
         <v>38</v>
       </c>
-      <c r="AM15" s="33"/>
     </row>
-    <row r="16" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A16" s="34">
+    <row r="16" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A16" s="28">
         <v>1</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30">
         <f t="shared" ref="C16:C23" si="0">SUM(D16:E16)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="37">
-        <f>SUM(H16,Y16,AC16,AG16,AK16)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="35">
-        <f t="shared" ref="E16:E23" si="1">SUM(M16,Z16,AD16,AH16,AL16)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="36">
-        <f t="shared" ref="F16:F23" si="2">SUM(H16,M16)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="38" t="e">
-        <f t="shared" ref="G16:G24" si="3">F16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="39">
-        <f t="shared" ref="H16:H23" si="4">SUM(I16:L16)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="39">
-        <f t="shared" ref="M16:M23" si="5">SUM(N16:Q16)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="37"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="40">
-        <f t="shared" ref="W16:W23" si="6">SUM(Y16:Z16)</f>
-        <v>0</v>
-      </c>
-      <c r="X16" s="41" t="e">
-        <f t="shared" ref="X16:X24" si="7">W16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="40">
-        <f t="shared" ref="AA16:AA23" si="8">SUM(AC16:AD16)</f>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="41" t="e">
-        <f t="shared" ref="AB16:AB24" si="9">AA16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="35"/>
-      <c r="AE16" s="40">
-        <f t="shared" ref="AE16:AE23" si="10">SUM(AG16:AH16)</f>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="41" t="e">
-        <f t="shared" ref="AF16:AF24" si="11">AE16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG16" s="37"/>
-      <c r="AH16" s="35"/>
-      <c r="AI16" s="40">
-        <f t="shared" ref="AI16:AI23" si="12">SUM(AK16:AL16)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="41" t="e">
-        <f t="shared" ref="AJ16:AJ24" si="13">AI16/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK16" s="37"/>
-      <c r="AL16" s="35"/>
-      <c r="AM16" s="33"/>
+      <c r="D16" s="31">
+        <f t="shared" ref="D16:D23" si="1">SUM(H16,Y16,AC16,AG16,AK16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" ref="E16:E23" si="2">SUM(M16,Z16,AD16,AH16,AL16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="30">
+        <f t="shared" ref="F16:F23" si="3">SUM(H16,M16)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="32" t="e">
+        <f t="shared" ref="G16:G24" si="4">F16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="33">
+        <f t="shared" ref="H16:H23" si="5">SUM(I16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="33">
+        <f t="shared" ref="M16:M23" si="6">SUM(N16:Q16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="34">
+        <f t="shared" ref="W16:W23" si="7">SUM(Y16:Z16)</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="35" t="e">
+        <f t="shared" ref="X16:X24" si="8">W16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="34">
+        <f t="shared" ref="AA16:AA23" si="9">SUM(AC16:AD16)</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="35" t="e">
+        <f t="shared" ref="AB16:AB24" si="10">AA16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="34">
+        <f t="shared" ref="AE16:AE23" si="11">SUM(AG16:AH16)</f>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="35" t="e">
+        <f t="shared" ref="AF16:AF24" si="12">AE16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG16" s="31"/>
+      <c r="AH16" s="29"/>
+      <c r="AI16" s="34">
+        <f t="shared" ref="AI16:AI23" si="13">SUM(AK16:AL16)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="35" t="e">
+        <f t="shared" ref="AJ16:AJ24" si="14">AI16/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK16" s="31"/>
+      <c r="AL16" s="29"/>
     </row>
-    <row r="17" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A17" s="34">
+    <row r="17" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A17" s="28">
         <v>2</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36">
+      <c r="B17" s="29"/>
+      <c r="C17" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D17" s="37">
-        <f t="shared" ref="D16:D23" si="14">SUM(H17,Y17,AC17,AG17,AK17)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="35">
+      <c r="D17" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17" s="36">
+      <c r="E17" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G17" s="38" t="e">
+      <c r="F17" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="39">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32" t="e">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="39">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="40">
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X17" s="41" t="e">
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="34">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="40">
+        <v>0</v>
+      </c>
+      <c r="X17" s="35" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="34">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC17" s="37"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="35" t="e">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF17" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="34">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG17" s="37"/>
-      <c r="AH17" s="35"/>
-      <c r="AI17" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="35" t="e">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="34">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK17" s="37"/>
-      <c r="AL17" s="35"/>
-      <c r="AM17" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="35" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK17" s="31"/>
+      <c r="AL17" s="29"/>
     </row>
-    <row r="18" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A18" s="34">
+    <row r="18" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A18" s="28">
         <v>3</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36">
+      <c r="B18" s="29"/>
+      <c r="C18" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="32" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="35" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="29"/>
+      <c r="AE18" s="34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="35" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="29"/>
+      <c r="AI18" s="34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="35" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="35">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="29"/>
+    </row>
+    <row r="19" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A19" s="28">
+        <v>4</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F18" s="36">
+      <c r="E19" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="38" t="e">
+      <c r="F19" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="39">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32" t="e">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="39">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="40">
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X18" s="41" t="e">
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="34">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="40">
+        <v>0</v>
+      </c>
+      <c r="X19" s="35" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="34">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="35" t="e">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF18" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="34">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG18" s="37"/>
-      <c r="AH18" s="35"/>
-      <c r="AI18" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="35" t="e">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG19" s="31"/>
+      <c r="AH19" s="29"/>
+      <c r="AI19" s="34">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK18" s="37"/>
-      <c r="AL18" s="35"/>
-      <c r="AM18" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="35" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK19" s="31"/>
+      <c r="AL19" s="29"/>
     </row>
-    <row r="19" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A19" s="34">
-        <v>4</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36">
+    <row r="20" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A20" s="28">
+        <v>5</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D20" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="32" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X20" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="35" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="29"/>
+      <c r="AE20" s="34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="35" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="29"/>
+      <c r="AI20" s="34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="35" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="35">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK20" s="31"/>
+      <c r="AL20" s="29"/>
+    </row>
+    <row r="21" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A21" s="28">
+        <v>6</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19" s="36">
+      <c r="E21" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G19" s="38" t="e">
+      <c r="F21" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="39">
+        <v>0</v>
+      </c>
+      <c r="G21" s="32" t="e">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="39">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="40">
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X19" s="41" t="e">
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="34">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="35"/>
-      <c r="AA19" s="40">
+        <v>0</v>
+      </c>
+      <c r="X21" s="35" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="34">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC19" s="37"/>
-      <c r="AD19" s="35"/>
-      <c r="AE19" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="35" t="e">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF19" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC21" s="31"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="34">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG19" s="37"/>
-      <c r="AH19" s="35"/>
-      <c r="AI19" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="35" t="e">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG21" s="31"/>
+      <c r="AH21" s="29"/>
+      <c r="AI21" s="34">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK19" s="37"/>
-      <c r="AL19" s="35"/>
-      <c r="AM19" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="35" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK21" s="31"/>
+      <c r="AL21" s="29"/>
     </row>
-    <row r="20" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A20" s="34">
-        <v>5</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36">
+    <row r="22" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A22" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D22" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="32" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X22" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="35" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="35" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG22" s="31"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="35" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="35">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK22" s="31"/>
+      <c r="AL22" s="29"/>
+    </row>
+    <row r="23" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A23" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F20" s="36">
+      <c r="E23" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G20" s="38" t="e">
+      <c r="F23" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="39">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32" t="e">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="39">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="40">
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X20" s="41" t="e">
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="34">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="35"/>
-      <c r="AA20" s="40">
+        <v>0</v>
+      </c>
+      <c r="X23" s="35" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="29"/>
+      <c r="AA23" s="34">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC20" s="37"/>
-      <c r="AD20" s="35"/>
-      <c r="AE20" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="35" t="e">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF20" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="34">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="35"/>
-      <c r="AI20" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="35" t="e">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="41" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG23" s="31"/>
+      <c r="AH23" s="29"/>
+      <c r="AI23" s="34">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK20" s="37"/>
-      <c r="AL20" s="35"/>
-      <c r="AM20" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="35" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK23" s="31"/>
+      <c r="AL23" s="29"/>
     </row>
-    <row r="21" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A21" s="34">
-        <v>6</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="37">
+    <row r="24" spans="1:38" ht="34.5" customHeight="1">
+      <c r="A24" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="37">
+        <f t="shared" ref="B24:F24" si="15">SUM(B16:B23)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="38">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="39">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="40">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="41">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="42" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="43">
+        <f t="shared" ref="H24:W24" si="16">SUM(H16:H23)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="43">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="40">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W24" s="41">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="42" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y24" s="43">
+        <f t="shared" ref="Y24:AA24" si="17">SUM(Y16:Y23)</f>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="40">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="41">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="42" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC24" s="43">
+        <f t="shared" ref="AC24:AE24" si="18">SUM(AC16:AC23)</f>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="40">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="41">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="42" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG24" s="43">
+        <f t="shared" ref="AG24:AI24" si="19">SUM(AG16:AG23)</f>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="40">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="41">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="42" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="38" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="39">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="40">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X21" s="41" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB21" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC21" s="37"/>
-      <c r="AD21" s="35"/>
-      <c r="AE21" s="40">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF21" s="41" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG21" s="37"/>
-      <c r="AH21" s="35"/>
-      <c r="AI21" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ21" s="41" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK21" s="37"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK24" s="43">
+        <f t="shared" ref="AK24:AL24" si="20">SUM(AK16:AK23)</f>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="40">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A22" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="37">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="38" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="39">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="40">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="41" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="35"/>
-      <c r="AA22" s="40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC22" s="37"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="40">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF22" s="41" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG22" s="37"/>
-      <c r="AH22" s="35"/>
-      <c r="AI22" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="41" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK22" s="37"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="33"/>
+    <row r="25" spans="1:38" ht="15" customHeight="1">
+      <c r="A25" s="44"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="45"/>
+      <c r="W25" s="45"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="45"/>
+      <c r="Z25" s="45"/>
+      <c r="AA25" s="45"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="45"/>
+      <c r="AD25" s="45"/>
+      <c r="AE25" s="45"/>
+      <c r="AF25" s="45"/>
+      <c r="AG25" s="45"/>
+      <c r="AH25" s="45"/>
+      <c r="AI25" s="45"/>
+      <c r="AJ25" s="46"/>
+      <c r="AK25" s="45"/>
+      <c r="AL25" s="45"/>
     </row>
-    <row r="23" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A23" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="37">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="38" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H23" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="39">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="40">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="41" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="35"/>
-      <c r="AA23" s="40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC23" s="37"/>
-      <c r="AD23" s="35"/>
-      <c r="AE23" s="40">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF23" s="41" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG23" s="37"/>
-      <c r="AH23" s="35"/>
-      <c r="AI23" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="41" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK23" s="37"/>
-      <c r="AL23" s="35"/>
-      <c r="AM23" s="33"/>
+    <row r="26" spans="1:38">
+      <c r="A26" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10"/>
+      <c r="AD26" s="10"/>
+      <c r="AE26" s="10"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="10"/>
+      <c r="AI26" s="10"/>
+      <c r="AJ26" s="10"/>
+      <c r="AK26" s="10"/>
+      <c r="AL26" s="10"/>
     </row>
-    <row r="24" spans="1:39" ht="34.5" customHeight="1">
-      <c r="A24" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="43">
-        <f t="shared" ref="B24:F24" si="15">SUM(B16:B23)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="44">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="45">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="46">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="47">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="48" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="49">
-        <f t="shared" ref="H24:W24" si="16">SUM(H16:H23)</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="S24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="T24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="U24" s="49">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="V24" s="46">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="W24" s="47">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="X24" s="48" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y24" s="49">
-        <f t="shared" ref="Y24:AA24" si="17">SUM(Y16:Y23)</f>
-        <v>0</v>
-      </c>
-      <c r="Z24" s="46">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AA24" s="47">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AB24" s="48" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC24" s="49">
-        <f t="shared" ref="AC24:AE24" si="18">SUM(AC16:AC23)</f>
-        <v>0</v>
-      </c>
-      <c r="AD24" s="46">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AE24" s="47">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AF24" s="48" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG24" s="49">
-        <f t="shared" ref="AG24:AI24" si="19">SUM(AG16:AG23)</f>
-        <v>0</v>
-      </c>
-      <c r="AH24" s="46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AI24" s="47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="48" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK24" s="49">
-        <f t="shared" ref="AK24:AL24" si="20">SUM(AK16:AK23)</f>
-        <v>0</v>
-      </c>
-      <c r="AL24" s="46">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AM24" s="33" t="e">
-        <f>SUM([1]SEREMBAN!AC19+[1]PD!AC19+[1]JEMPOL!AC19+[1]TAMPIN!AC19+[1]JELEBU!AC19+[1]K.PILAH!AC19+[1]REMBAU!AC19+#REF!+#REF!+#REF!+#REF!+#REF!)</f>
-        <v>#REF!</v>
-      </c>
+    <row r="27" spans="1:38">
+      <c r="A27" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="49"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="10"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="10"/>
+      <c r="AJ27" s="10"/>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="10"/>
     </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="52"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="51"/>
-      <c r="AA25" s="51"/>
-      <c r="AB25" s="52"/>
-      <c r="AC25" s="51"/>
-      <c r="AD25" s="51"/>
-      <c r="AE25" s="51"/>
-      <c r="AF25" s="51"/>
-      <c r="AG25" s="51"/>
-      <c r="AH25" s="51"/>
-      <c r="AI25" s="51"/>
-      <c r="AJ25" s="52"/>
-      <c r="AK25" s="51"/>
-      <c r="AL25" s="51"/>
-      <c r="AM25" s="53"/>
+    <row r="28" spans="1:38">
+      <c r="A28" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
     </row>
-    <row r="26" spans="1:39">
-      <c r="A26" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="11"/>
-      <c r="AC26" s="11"/>
-      <c r="AD26" s="11"/>
-      <c r="AE26" s="11"/>
-      <c r="AF26" s="11"/>
-      <c r="AG26" s="11"/>
-      <c r="AH26" s="11"/>
-      <c r="AI26" s="11"/>
-      <c r="AJ26" s="11"/>
-      <c r="AK26" s="11"/>
-      <c r="AL26" s="11"/>
-      <c r="AM26" s="11"/>
+    <row r="29" spans="1:38">
+      <c r="A29" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
     </row>
-    <row r="27" spans="1:39">
-      <c r="A27" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AL27" s="11"/>
-      <c r="AM27" s="11"/>
+    <row r="30" spans="1:38">
+      <c r="A30" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="50"/>
+      <c r="AC30" s="50"/>
+      <c r="AD30" s="50"/>
+      <c r="AE30" s="50"/>
+      <c r="AF30" s="50"/>
+      <c r="AG30" s="50"/>
+      <c r="AH30" s="50"/>
+      <c r="AI30" s="54"/>
+      <c r="AJ30" s="54"/>
+      <c r="AK30" s="54"/>
+      <c r="AL30" s="54"/>
     </row>
-    <row r="28" spans="1:39">
-      <c r="A28" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
+    <row r="31" spans="1:38" ht="19.5" customHeight="1">
+      <c r="A31" s="50"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="50"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="50"/>
+      <c r="Z31" s="50"/>
+      <c r="AA31" s="50"/>
+      <c r="AB31" s="50"/>
+      <c r="AC31" s="50"/>
+      <c r="AD31" s="50"/>
+      <c r="AE31" s="50"/>
+      <c r="AF31" s="50"/>
+      <c r="AG31" s="50"/>
+      <c r="AH31" s="50"/>
+      <c r="AI31" s="54"/>
+      <c r="AJ31" s="54"/>
+      <c r="AK31" s="54"/>
+      <c r="AL31" s="54"/>
     </row>
-    <row r="29" spans="1:39">
-      <c r="A29" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-    </row>
-    <row r="30" spans="1:39">
-      <c r="A30" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="57"/>
-      <c r="P30" s="57"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="57"/>
-      <c r="S30" s="57"/>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="V30" s="57"/>
-      <c r="W30" s="57"/>
-      <c r="X30" s="57"/>
-      <c r="Y30" s="57"/>
-      <c r="Z30" s="57"/>
-      <c r="AA30" s="57"/>
-      <c r="AB30" s="57"/>
-      <c r="AC30" s="57"/>
-      <c r="AD30" s="57"/>
-      <c r="AE30" s="57"/>
-      <c r="AF30" s="57"/>
-      <c r="AG30" s="57"/>
-      <c r="AH30" s="57"/>
-      <c r="AI30" s="61"/>
-      <c r="AJ30" s="61"/>
-      <c r="AK30" s="61"/>
-      <c r="AL30" s="61"/>
-      <c r="AM30" s="61"/>
-    </row>
-    <row r="31" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="57"/>
-      <c r="R31" s="57"/>
-      <c r="S31" s="57"/>
-      <c r="T31" s="57"/>
-      <c r="U31" s="57"/>
-      <c r="V31" s="57"/>
-      <c r="W31" s="57"/>
-      <c r="X31" s="57"/>
-      <c r="Y31" s="57"/>
-      <c r="Z31" s="57"/>
-      <c r="AA31" s="57"/>
-      <c r="AB31" s="57"/>
-      <c r="AC31" s="57"/>
-      <c r="AD31" s="57"/>
-      <c r="AE31" s="57"/>
-      <c r="AF31" s="57"/>
-      <c r="AG31" s="57"/>
-      <c r="AH31" s="57"/>
-      <c r="AI31" s="61"/>
-      <c r="AJ31" s="61"/>
-      <c r="AK31" s="61"/>
-      <c r="AL31" s="61"/>
-      <c r="AM31" s="61"/>
-    </row>
-    <row r="32" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A32" s="57"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="61"/>
-      <c r="P32" s="61"/>
-      <c r="Q32" s="61"/>
-      <c r="R32" s="61"/>
-      <c r="S32" s="61"/>
-      <c r="T32" s="61"/>
-      <c r="U32" s="61"/>
-      <c r="V32" s="61"/>
-      <c r="W32" s="61"/>
-      <c r="X32" s="61"/>
-      <c r="Y32" s="61"/>
-      <c r="Z32" s="61"/>
-      <c r="AA32" s="61"/>
-      <c r="AB32" s="61"/>
-      <c r="AC32" s="61"/>
-      <c r="AD32" s="61"/>
-      <c r="AE32" s="61"/>
-      <c r="AF32" s="61"/>
-      <c r="AG32" s="61"/>
-      <c r="AH32" s="61"/>
-      <c r="AI32" s="61"/>
-      <c r="AJ32" s="61"/>
-      <c r="AK32" s="61"/>
-      <c r="AL32" s="61"/>
-      <c r="AM32" s="61"/>
+    <row r="32" spans="1:38" ht="19.5" customHeight="1">
+      <c r="A32" s="50"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
+      <c r="T32" s="54"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="54"/>
+      <c r="W32" s="54"/>
+      <c r="X32" s="54"/>
+      <c r="Y32" s="54"/>
+      <c r="Z32" s="54"/>
+      <c r="AA32" s="54"/>
+      <c r="AB32" s="54"/>
+      <c r="AC32" s="54"/>
+      <c r="AD32" s="54"/>
+      <c r="AE32" s="54"/>
+      <c r="AF32" s="54"/>
+      <c r="AG32" s="54"/>
+      <c r="AH32" s="54"/>
+      <c r="AI32" s="54"/>
+      <c r="AJ32" s="54"/>
+      <c r="AK32" s="54"/>
+      <c r="AL32" s="54"/>
     </row>
     <row r="33" spans="2:29" ht="15" customHeight="1">
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="63"/>
-      <c r="U33" s="63"/>
-      <c r="V33" s="63"/>
-      <c r="W33" s="63"/>
-      <c r="X33" s="63"/>
-      <c r="Y33" s="63"/>
-      <c r="Z33" s="63"/>
-      <c r="AA33" s="63"/>
-      <c r="AB33" s="63"/>
-      <c r="AC33" s="63"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="56"/>
+      <c r="U33" s="56"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="56"/>
+      <c r="Y33" s="56"/>
+      <c r="Z33" s="56"/>
+      <c r="AA33" s="56"/>
+      <c r="AB33" s="56"/>
+      <c r="AC33" s="56"/>
     </row>
     <row r="34" spans="2:29" ht="15.75" customHeight="1"/>
     <row r="35" spans="2:29" ht="15.75" customHeight="1"/>
@@ -4135,7 +4051,7 @@
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="A3:AL3"/>
-    <mergeCell ref="A4:AM4"/>
+    <mergeCell ref="A4:AL4"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="S5:T5"/>

</xml_diff>